<commit_message>
feat: Update UI components for consistent styling and enhance service management with new sample subclass functionality
</commit_message>
<xml_diff>
--- a/src/features/customer/services/data/services.xlsx
+++ b/src/features/customer/services/data/services.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Desktop/projects/gims/src/features/customer/services/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{44C6B395-B669-CB48-B8BB-F756BA8678B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7956316-B625-024B-867D-AA5D6BFC44A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="680" windowWidth="29920" windowHeight="17620" activeTab="3" xr2:uid="{EC5FDFC6-30BD-4E71-B1E7-A44EE30A6994}"/>
+    <workbookView xWindow="15300" yWindow="680" windowWidth="14620" windowHeight="17180" activeTab="3" xr2:uid="{EC5FDFC6-30BD-4E71-B1E7-A44EE30A6994}"/>
   </bookViews>
   <sheets>
     <sheet name="Aggregates" sheetId="5" r:id="rId1"/>
@@ -2417,9 +2417,6 @@
     <t>Evaluation of Flexural Strength</t>
   </si>
   <si>
-    <t>BS ISO 1920-14:2019, BS EN 480-</t>
-  </si>
-  <si>
     <t>ASTM C143-15</t>
   </si>
   <si>
@@ -2859,6 +2856,9 @@
   </si>
   <si>
     <t>Water</t>
+  </si>
+  <si>
+    <t>BS ISO 1920-14:2019, BS EN 480-2:2006</t>
   </si>
 </sst>
 </file>
@@ -3011,7 +3011,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -3078,11 +3078,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3401,8 +3400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{097ACAEE-3120-3A46-8319-40D9260ED962}">
   <dimension ref="A1:H108"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView topLeftCell="A89" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3422,7 +3421,7 @@
       <c r="B1" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>197</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -3431,35 +3430,35 @@
       <c r="E1" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="22" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B2" s="16" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="17" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="D2" s="17" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="E2" s="18"/>
       <c r="G2" s="2" t="s">
+        <v>912</v>
+      </c>
+      <c r="H2" s="2" t="s">
         <v>913</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B3" s="16" t="s">
         <v>1</v>
@@ -3468,19 +3467,19 @@
         <v>204</v>
       </c>
       <c r="D3" s="17" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="E3" s="18"/>
       <c r="G3" s="2" t="s">
         <v>412</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>2</v>
@@ -3489,19 +3488,19 @@
         <v>204</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="E4" s="18"/>
       <c r="G4" s="2" t="s">
         <v>410</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>3</v>
@@ -3510,19 +3509,19 @@
         <v>204</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="E5" s="19"/>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="2" t="s">
+        <v>916</v>
+      </c>
+      <c r="H5" s="2" t="s">
         <v>917</v>
-      </c>
-      <c r="H5" s="29" t="s">
-        <v>918</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>4</v>
@@ -3531,7 +3530,7 @@
         <v>204</v>
       </c>
       <c r="D6" s="17" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="E6" s="18"/>
       <c r="G6" s="14"/>
@@ -3539,7 +3538,7 @@
     </row>
     <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>5</v>
@@ -3548,7 +3547,7 @@
         <v>204</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="E7" s="18"/>
       <c r="G7" s="14"/>
@@ -3556,7 +3555,7 @@
     </row>
     <row r="8" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>6</v>
@@ -3565,13 +3564,13 @@
         <v>204</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="E8" s="18"/>
     </row>
     <row r="9" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>7</v>
@@ -3580,13 +3579,13 @@
         <v>204</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="E9" s="18"/>
     </row>
     <row r="10" spans="1:8" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B10" s="16" t="s">
         <v>8</v>
@@ -3595,7 +3594,7 @@
         <v>204</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="E10" s="18"/>
     </row>
@@ -3610,7 +3609,7 @@
         <v>204</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="E11" s="18"/>
     </row>
@@ -3625,7 +3624,7 @@
         <v>204</v>
       </c>
       <c r="D12" s="17" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="E12" s="18"/>
     </row>
@@ -3640,7 +3639,7 @@
         <v>204</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="E13" s="18"/>
     </row>
@@ -3655,7 +3654,7 @@
         <v>204</v>
       </c>
       <c r="D14" s="17" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E14" s="18"/>
     </row>
@@ -3670,7 +3669,7 @@
         <v>204</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="E15" s="18"/>
     </row>
@@ -3685,7 +3684,7 @@
         <v>204</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E16" s="18"/>
     </row>
@@ -3700,7 +3699,7 @@
         <v>204</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="E17" s="18"/>
     </row>
@@ -3715,7 +3714,7 @@
         <v>204</v>
       </c>
       <c r="D18" s="17" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="E18" s="18"/>
     </row>
@@ -3730,7 +3729,7 @@
         <v>204</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="E19" s="18"/>
     </row>
@@ -3742,10 +3741,10 @@
         <v>18</v>
       </c>
       <c r="C20" s="17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="D20" s="17" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="E20" s="18"/>
     </row>
@@ -3760,7 +3759,7 @@
         <v>204</v>
       </c>
       <c r="D21" s="17" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="E21" s="18"/>
     </row>
@@ -3775,7 +3774,7 @@
         <v>204</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="E22" s="18"/>
     </row>
@@ -3790,7 +3789,7 @@
         <v>204</v>
       </c>
       <c r="D23" s="17" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="E23" s="18"/>
     </row>
@@ -3820,7 +3819,7 @@
         <v>356</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="E25" s="18"/>
     </row>
@@ -3847,7 +3846,7 @@
         <v>39</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>204</v>
@@ -3937,7 +3936,7 @@
         <v>48</v>
       </c>
       <c r="C33" s="20" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>364</v>
@@ -3955,7 +3954,7 @@
         <v>204</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E34" s="18"/>
     </row>
@@ -3970,7 +3969,7 @@
         <v>204</v>
       </c>
       <c r="D35" s="17" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="E35" s="19"/>
     </row>
@@ -3985,7 +3984,7 @@
         <v>204</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E36" s="18"/>
     </row>
@@ -4000,7 +3999,7 @@
         <v>204</v>
       </c>
       <c r="D37" s="17" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="E37" s="18"/>
     </row>
@@ -4030,7 +4029,7 @@
         <v>204</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="E39" s="18"/>
     </row>
@@ -4045,7 +4044,7 @@
         <v>204</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E40" s="18"/>
     </row>
@@ -4060,7 +4059,7 @@
         <v>204</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E41" s="18"/>
     </row>
@@ -4087,7 +4086,7 @@
         <v>58</v>
       </c>
       <c r="C43" s="25" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D43" s="17" t="s">
         <v>204</v>
@@ -4102,10 +4101,10 @@
         <v>59</v>
       </c>
       <c r="C44" s="25" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D44" s="17" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="E44" s="18"/>
     </row>
@@ -4117,7 +4116,7 @@
         <v>60</v>
       </c>
       <c r="C45" s="25" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="D45" s="17" t="s">
         <v>204</v>
@@ -4132,10 +4131,10 @@
         <v>61</v>
       </c>
       <c r="C46" s="20" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="E46" s="18"/>
     </row>
@@ -4237,7 +4236,7 @@
         <v>86</v>
       </c>
       <c r="C53" s="17" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D53" s="17" t="s">
         <v>204</v>
@@ -4360,7 +4359,7 @@
         <v>204</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="E61" s="18"/>
     </row>
@@ -4495,7 +4494,7 @@
         <v>204</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="E70" s="18"/>
     </row>
@@ -4552,7 +4551,7 @@
         <v>113</v>
       </c>
       <c r="C74" s="20" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="D74" s="17" t="s">
         <v>204</v>
@@ -4570,7 +4569,7 @@
         <v>204</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="E75" s="18"/>
     </row>
@@ -4585,7 +4584,7 @@
         <v>382</v>
       </c>
       <c r="D76" s="17" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="E76" s="18"/>
     </row>
@@ -4627,7 +4626,7 @@
         <v>133</v>
       </c>
       <c r="C79" s="17" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="D79" s="17" t="s">
         <v>204</v>
@@ -4642,7 +4641,7 @@
         <v>134</v>
       </c>
       <c r="C80" s="20" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="D80" s="17" t="s">
         <v>204</v>
@@ -4660,7 +4659,7 @@
         <v>204</v>
       </c>
       <c r="D81" s="17" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="E81" s="18"/>
     </row>
@@ -4672,7 +4671,7 @@
         <v>143</v>
       </c>
       <c r="C82" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D82" s="21"/>
       <c r="E82" s="18"/>
@@ -4685,7 +4684,7 @@
         <v>144</v>
       </c>
       <c r="C83" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D83" s="21"/>
       <c r="E83" s="18"/>
@@ -4698,7 +4697,7 @@
         <v>145</v>
       </c>
       <c r="C84" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D84" s="21"/>
       <c r="E84" s="18"/>
@@ -4711,7 +4710,7 @@
         <v>146</v>
       </c>
       <c r="C85" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D85" s="21"/>
       <c r="E85" s="18"/>
@@ -4724,7 +4723,7 @@
         <v>147</v>
       </c>
       <c r="C86" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D86" s="3"/>
       <c r="E86" s="19"/>
@@ -4737,7 +4736,7 @@
         <v>148</v>
       </c>
       <c r="C87" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D87" s="21"/>
       <c r="E87" s="18"/>
@@ -4750,7 +4749,7 @@
         <v>149</v>
       </c>
       <c r="C88" s="9" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D88" s="21"/>
       <c r="E88" s="18"/>
@@ -4763,7 +4762,7 @@
         <v>150</v>
       </c>
       <c r="C89" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D89" s="3"/>
       <c r="E89" s="19"/>
@@ -4776,7 +4775,7 @@
         <v>111</v>
       </c>
       <c r="C90" s="17" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D90" s="21"/>
       <c r="E90" s="18"/>
@@ -4789,7 +4788,7 @@
         <v>112</v>
       </c>
       <c r="C91" s="9" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="D91" s="21"/>
       <c r="E91" s="18"/>
@@ -4802,7 +4801,7 @@
         <v>151</v>
       </c>
       <c r="C92" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D92" s="21"/>
       <c r="E92" s="18"/>
@@ -4815,7 +4814,7 @@
         <v>152</v>
       </c>
       <c r="C93" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D93" s="3"/>
       <c r="E93" s="19"/>
@@ -4828,7 +4827,7 @@
         <v>153</v>
       </c>
       <c r="C94" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D94" s="21"/>
       <c r="E94" s="18"/>
@@ -4841,7 +4840,7 @@
         <v>154</v>
       </c>
       <c r="C95" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D95" s="21"/>
       <c r="E95" s="18"/>
@@ -4854,7 +4853,7 @@
         <v>155</v>
       </c>
       <c r="C96" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D96" s="3"/>
       <c r="E96" s="19"/>
@@ -4867,7 +4866,7 @@
         <v>156</v>
       </c>
       <c r="C97" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D97" s="21"/>
       <c r="E97" s="18"/>
@@ -4880,7 +4879,7 @@
         <v>157</v>
       </c>
       <c r="C98" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D98" s="21"/>
       <c r="E98" s="18"/>
@@ -4893,7 +4892,7 @@
         <v>158</v>
       </c>
       <c r="C99" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D99" s="21"/>
       <c r="E99" s="18"/>
@@ -4906,7 +4905,7 @@
         <v>159</v>
       </c>
       <c r="C100" s="17" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="D100" s="3"/>
       <c r="E100" s="19"/>
@@ -4919,7 +4918,7 @@
         <v>160</v>
       </c>
       <c r="C101" s="17" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D101" s="21"/>
       <c r="E101" s="18"/>
@@ -4932,7 +4931,7 @@
         <v>161</v>
       </c>
       <c r="C102" s="17" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="D102" s="21"/>
       <c r="E102" s="18"/>
@@ -4948,7 +4947,7 @@
         <v>204</v>
       </c>
       <c r="D103" s="17" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="E103" s="18"/>
     </row>
@@ -4973,7 +4972,7 @@
         <v>164</v>
       </c>
       <c r="C105" s="9" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="D105" s="21"/>
       <c r="E105" s="18"/>
@@ -4986,7 +4985,7 @@
         <v>165</v>
       </c>
       <c r="C106" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D106" s="3"/>
       <c r="E106" s="19"/>
@@ -4999,7 +4998,7 @@
         <v>166</v>
       </c>
       <c r="C107" s="17" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="D107" s="3"/>
       <c r="E107" s="19"/>
@@ -5012,7 +5011,7 @@
         <v>167</v>
       </c>
       <c r="C108" s="17" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="D108" s="21"/>
       <c r="E108" s="18"/>
@@ -5031,8 +5030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B234315E-79C9-AE41-96FF-8B7B0AC7EA1D}">
   <dimension ref="A1:H87"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5061,10 +5060,10 @@
       <c r="E1" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -5197,7 +5196,7 @@
         <v>209</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>210</v>
@@ -6409,8 +6408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72593B9F-5EF7-F748-A291-E34DBB51C9CD}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView topLeftCell="B39" zoomScale="101" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6439,10 +6438,10 @@
       <c r="E1" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -7488,13 +7487,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{64C4F372-8830-8348-B95A-9274D57190A6}">
   <dimension ref="A1:H86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:XFD9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="15" customWidth="1"/>
     <col min="2" max="2" width="64.83203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31" customWidth="1"/>
+    <col min="3" max="3" width="35.6640625" customWidth="1"/>
     <col min="4" max="4" width="31.5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.83203125" customWidth="1"/>
     <col min="8" max="8" width="33.6640625" bestFit="1" customWidth="1"/>
@@ -7507,7 +7508,7 @@
       <c r="B1" s="27" t="s">
         <v>196</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="28" t="s">
         <v>197</v>
       </c>
       <c r="D1" s="27" t="s">
@@ -7516,10 +7517,10 @@
       <c r="E1" s="27" t="s">
         <v>199</v>
       </c>
-      <c r="G1" s="28" t="s">
+      <c r="G1" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="H1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
@@ -7536,10 +7537,10 @@
       </c>
       <c r="E2" s="10"/>
       <c r="G2" s="2" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7557,10 +7558,10 @@
       </c>
       <c r="E3" s="10"/>
       <c r="G3" s="2" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7578,10 +7579,10 @@
       </c>
       <c r="E4" s="10"/>
       <c r="G4" s="2" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7599,10 +7600,10 @@
       </c>
       <c r="E5" s="10"/>
       <c r="G5" s="2" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7620,10 +7621,10 @@
       </c>
       <c r="E6" s="10"/>
       <c r="G6" s="2" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7641,10 +7642,10 @@
       </c>
       <c r="E7" s="10"/>
       <c r="G7" s="2" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="17" x14ac:dyDescent="0.2">
@@ -7802,7 +7803,7 @@
         <v>646</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>381</v>
@@ -7985,7 +7986,7 @@
         <v>669</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>789</v>
+        <v>918</v>
       </c>
       <c r="D30" s="9" t="s">
         <v>670</v>
@@ -8033,7 +8034,7 @@
         <v>636</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="E33" s="10"/>
     </row>
@@ -8057,7 +8058,7 @@
         <v>678</v>
       </c>
       <c r="B35" s="9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C35" s="9" t="s">
         <v>679</v>
@@ -8117,13 +8118,13 @@
         <v>688</v>
       </c>
       <c r="B39" s="9" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>685</v>
       </c>
       <c r="D39" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E39" s="10"/>
     </row>
@@ -8132,13 +8133,13 @@
         <v>689</v>
       </c>
       <c r="B40" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C40" s="9" t="s">
         <v>685</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E40" s="10"/>
     </row>
@@ -8153,7 +8154,7 @@
         <v>692</v>
       </c>
       <c r="D41" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E41" s="10"/>
     </row>
@@ -8168,7 +8169,7 @@
         <v>692</v>
       </c>
       <c r="D42" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E42" s="10"/>
     </row>
@@ -8183,7 +8184,7 @@
         <v>692</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="E43" s="10"/>
     </row>
@@ -8192,7 +8193,7 @@
         <v>697</v>
       </c>
       <c r="B44" s="9" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C44" s="9" t="s">
         <v>692</v>
@@ -8207,7 +8208,7 @@
         <v>698</v>
       </c>
       <c r="B45" s="9" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C45" s="9" t="s">
         <v>692</v>
@@ -8222,13 +8223,13 @@
         <v>699</v>
       </c>
       <c r="B46" s="9" t="s">
+        <v>796</v>
+      </c>
+      <c r="C46" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D46" s="9" t="s">
         <v>797</v>
-      </c>
-      <c r="C46" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D46" s="9" t="s">
-        <v>798</v>
       </c>
       <c r="E46" s="10"/>
     </row>
@@ -8237,7 +8238,7 @@
         <v>700</v>
       </c>
       <c r="B47" s="9" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C47" s="9" t="s">
         <v>701</v>
@@ -8252,7 +8253,7 @@
         <v>702</v>
       </c>
       <c r="B48" s="9" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C48" s="9" t="s">
         <v>701</v>
@@ -8267,7 +8268,7 @@
         <v>703</v>
       </c>
       <c r="B49" s="9" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C49" s="9" t="s">
         <v>701</v>
@@ -8282,10 +8283,10 @@
         <v>704</v>
       </c>
       <c r="B50" s="9" t="s">
+        <v>800</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>801</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>802</v>
       </c>
       <c r="D50" s="9" t="s">
         <v>204</v>
@@ -8297,10 +8298,10 @@
         <v>705</v>
       </c>
       <c r="B51" s="9" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C51" s="9" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="D51" s="9" t="s">
         <v>204</v>
@@ -8312,10 +8313,10 @@
         <v>707</v>
       </c>
       <c r="B52" s="9" t="s">
+        <v>803</v>
+      </c>
+      <c r="C52" s="9" t="s">
         <v>804</v>
-      </c>
-      <c r="C52" s="9" t="s">
-        <v>805</v>
       </c>
       <c r="D52" s="9" t="s">
         <v>204</v>
@@ -8327,13 +8328,13 @@
         <v>708</v>
       </c>
       <c r="B53" s="9" t="s">
+        <v>805</v>
+      </c>
+      <c r="C53" s="9" t="s">
+        <v>204</v>
+      </c>
+      <c r="D53" s="9" t="s">
         <v>806</v>
-      </c>
-      <c r="C53" s="9" t="s">
-        <v>204</v>
-      </c>
-      <c r="D53" s="9" t="s">
-        <v>807</v>
       </c>
       <c r="E53" s="10"/>
     </row>
@@ -8342,7 +8343,7 @@
         <v>709</v>
       </c>
       <c r="B54" s="9" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C54" s="9" t="s">
         <v>710</v>
@@ -8357,13 +8358,13 @@
         <v>711</v>
       </c>
       <c r="B55" s="9" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C55" s="9" t="s">
         <v>204</v>
       </c>
       <c r="D55" s="9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E55" s="10"/>
     </row>
@@ -8372,10 +8373,10 @@
         <v>712</v>
       </c>
       <c r="B56" s="9" t="s">
+        <v>809</v>
+      </c>
+      <c r="C56" s="9" t="s">
         <v>810</v>
-      </c>
-      <c r="C56" s="9" t="s">
-        <v>811</v>
       </c>
       <c r="D56" s="9" t="s">
         <v>204</v>
@@ -8387,10 +8388,10 @@
         <v>713</v>
       </c>
       <c r="B57" s="9" t="s">
+        <v>811</v>
+      </c>
+      <c r="C57" s="9" t="s">
         <v>812</v>
-      </c>
-      <c r="C57" s="9" t="s">
-        <v>813</v>
       </c>
       <c r="D57" s="9" t="s">
         <v>204</v>
@@ -8402,10 +8403,10 @@
         <v>714</v>
       </c>
       <c r="B58" s="9" t="s">
+        <v>813</v>
+      </c>
+      <c r="C58" s="9" t="s">
         <v>814</v>
-      </c>
-      <c r="C58" s="9" t="s">
-        <v>815</v>
       </c>
       <c r="D58" s="9" t="s">
         <v>204</v>
@@ -8417,10 +8418,10 @@
         <v>715</v>
       </c>
       <c r="B59" s="9" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C59" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D59" s="9" t="s">
         <v>204</v>
@@ -8435,7 +8436,7 @@
         <v>717</v>
       </c>
       <c r="C60" s="9" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D60" s="9" t="s">
         <v>204</v>
@@ -8447,13 +8448,13 @@
         <v>718</v>
       </c>
       <c r="B61" s="9" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C61" s="9" t="s">
         <v>204</v>
       </c>
       <c r="D61" s="9" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E61" s="10"/>
     </row>
@@ -8468,7 +8469,7 @@
         <v>204</v>
       </c>
       <c r="D62" s="9" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="E62" s="10"/>
     </row>
@@ -8477,13 +8478,13 @@
         <v>721</v>
       </c>
       <c r="B63" s="9" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C63" s="9" t="s">
         <v>204</v>
       </c>
       <c r="D63" s="9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E63" s="10"/>
     </row>
@@ -8492,13 +8493,13 @@
         <v>722</v>
       </c>
       <c r="B64" s="9" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C64" s="9" t="s">
         <v>204</v>
       </c>
       <c r="D64" s="9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E64" s="10"/>
     </row>
@@ -8507,13 +8508,13 @@
         <v>723</v>
       </c>
       <c r="B65" s="9" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C65" s="9" t="s">
         <v>204</v>
       </c>
       <c r="D65" s="9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E65" s="10"/>
     </row>
@@ -8528,7 +8529,7 @@
         <v>204</v>
       </c>
       <c r="D66" s="9" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="E66" s="10"/>
     </row>
@@ -8537,13 +8538,13 @@
         <v>726</v>
       </c>
       <c r="B67" s="9" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C67" s="9" t="s">
         <v>727</v>
       </c>
       <c r="D67" s="9" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="E67" s="10"/>
     </row>
@@ -8558,7 +8559,7 @@
         <v>730</v>
       </c>
       <c r="D68" s="9" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="E68" s="10"/>
     </row>
@@ -8573,7 +8574,7 @@
         <v>727</v>
       </c>
       <c r="D69" s="9" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="E69" s="10"/>
     </row>
@@ -8588,7 +8589,7 @@
         <v>735</v>
       </c>
       <c r="D70" s="9" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="E70" s="10"/>
     </row>
@@ -8603,7 +8604,7 @@
         <v>735</v>
       </c>
       <c r="D71" s="9" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="E71" s="10"/>
     </row>
@@ -8657,13 +8658,13 @@
         <v>743</v>
       </c>
       <c r="B75" s="9" t="s">
+        <v>826</v>
+      </c>
+      <c r="C75" s="9" t="s">
         <v>827</v>
       </c>
-      <c r="C75" s="9" t="s">
-        <v>828</v>
-      </c>
       <c r="D75" s="9" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="E75" s="10"/>
     </row>
@@ -8678,7 +8679,7 @@
         <v>746</v>
       </c>
       <c r="D76" s="9" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="E76" s="10"/>
     </row>
@@ -8687,13 +8688,13 @@
         <v>747</v>
       </c>
       <c r="B77" s="9" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C77" s="9" t="s">
         <v>746</v>
       </c>
       <c r="D77" s="9" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="E77" s="10"/>
     </row>
@@ -8708,7 +8709,7 @@
         <v>746</v>
       </c>
       <c r="D78" s="9" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="E78" s="10"/>
     </row>
@@ -8717,10 +8718,10 @@
         <v>750</v>
       </c>
       <c r="B79" s="9" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C79" s="9" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D79" s="9" t="s">
         <v>204</v>
@@ -8732,10 +8733,10 @@
         <v>751</v>
       </c>
       <c r="B80" s="9" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C80" s="9" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D80" s="9" t="s">
         <v>752</v>
@@ -8747,10 +8748,10 @@
         <v>753</v>
       </c>
       <c r="B81" s="9" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C81" s="9" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D81" s="9" t="s">
         <v>752</v>
@@ -8765,7 +8766,7 @@
         <v>755</v>
       </c>
       <c r="C82" s="9" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D82" s="9" t="s">
         <v>204</v>
@@ -8777,10 +8778,10 @@
         <v>756</v>
       </c>
       <c r="B83" s="9" t="s">
+        <v>838</v>
+      </c>
+      <c r="C83" s="9" t="s">
         <v>839</v>
-      </c>
-      <c r="C83" s="9" t="s">
-        <v>840</v>
       </c>
       <c r="D83" s="9" t="s">
         <v>204</v>
@@ -8795,7 +8796,7 @@
         <v>758</v>
       </c>
       <c r="C84" s="9" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D84" s="9" t="s">
         <v>204</v>
@@ -8807,10 +8808,10 @@
         <v>759</v>
       </c>
       <c r="B85" s="9" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C85" s="9" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D85" s="9" t="s">
         <v>204</v>
@@ -8825,7 +8826,7 @@
         <v>761</v>
       </c>
       <c r="C86" s="9" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D86" s="9" t="s">
         <v>204</v>

</xml_diff>